<commit_message>
update test_suite _excelRead log
</commit_message>
<xml_diff>
--- a/testData/login_test_data.xlsx
+++ b/testData/login_test_data.xlsx
@@ -47,34 +47,42 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
+    <t>isomper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>口令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ccc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆时输入初始化用户能够正常登陆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆时输入新添加的用户和口令能够正常登陆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>isomper</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>口令</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登陆方式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>检查点</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ccc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>测试点说明</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -83,15 +91,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>登陆时输入初始化用户能够正常登陆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登陆时输入新添加的用户和口令能够正常登陆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>账号或口令错误</t>
+    <t>账号或口令错误1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -509,9 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -522,31 +520,31 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -554,14 +552,14 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -569,7 +567,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -578,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>

</xml_diff>